<commit_message>
Đoàn đẩy tai lieu va sua cai file bieu mau
</commit_message>
<xml_diff>
--- a/Document/2.Design/Template/Thong_tin_chi_tiet_hang_trong_kho.xlsx
+++ b/Document/2.Design/Template/Thong_tin_chi_tiet_hang_trong_kho.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="340"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" tabRatio="340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -105,12 +105,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -118,7 +118,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -126,7 +126,7 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -140,12 +140,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -153,45 +153,39 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -476,124 +470,156 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="33.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" customWidth="1"/>
-    <col min="7" max="7" width="24" style="6" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" style="6" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.25" style="8" customWidth="1"/>
+    <col min="2" max="2" width="18.875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="33.375" style="8" customWidth="1"/>
+    <col min="4" max="4" width="14.75" style="8" customWidth="1"/>
+    <col min="5" max="5" width="18" style="8" customWidth="1"/>
+    <col min="6" max="6" width="23.625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="24" style="9" customWidth="1"/>
+    <col min="8" max="8" width="18.625" style="9" customWidth="1"/>
+    <col min="9" max="9" width="18.125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:9" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+    </row>
+    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2"/>
+      <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="D2"/>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3"/>
+      <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="D3"/>
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4"/>
+      <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="D4"/>
+      <c r="E4"/>
+      <c r="F4"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5"/>
+      <c r="B5"/>
+      <c r="C5"/>
+      <c r="D5"/>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:9" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="I8" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>